<commit_message>
Add: Template for excel sheet
</commit_message>
<xml_diff>
--- a/src/calculator/templates/calculator/Template.xlsx
+++ b/src/calculator/templates/calculator/Template.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaio/Workspace/python/MacroCal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaio/Workspace/python/MacroCal/src/calculator/templates/calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2BCE766-6565-FE4C-84B2-CD4D7F18CD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229BC510-A148-9348-8488-7BC912965F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="1260" windowWidth="33640" windowHeight="20600" xr2:uid="{E1F56209-5FDF-9940-87DD-7244E19B7075}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,9 +47,6 @@
     <t>Weight kg</t>
   </si>
   <si>
-    <t>Height lb</t>
-  </si>
-  <si>
     <t>Weight lb</t>
   </si>
   <si>
@@ -63,13 +60,21 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Height cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0\ &quot;kg&quot;"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;lb&quot;"/>
+    <numFmt numFmtId="166" formatCode="0\ &quot;cm&quot;"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,16 +82,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,12 +112,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,10 +172,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,46 +471,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5F391E-9C8D-754D-A0AE-FCA2F4447B2C}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="5" customWidth="1"/>
+    <col min="2" max="3" width="9.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: Sheets for different macro distributions
</commit_message>
<xml_diff>
--- a/src/calculator/templates/calculator/Template.xlsx
+++ b/src/calculator/templates/calculator/Template.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaio/Workspace/python/MacroCal/src/calculator/templates/calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229BC510-A148-9348-8488-7BC912965F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1BEFBF-5B8F-8C46-AFAE-66D8705386ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="1260" windowWidth="33640" windowHeight="20600" xr2:uid="{E1F56209-5FDF-9940-87DD-7244E19B7075}"/>
+    <workbookView xWindow="280" yWindow="1260" windowWidth="33640" windowHeight="20600" activeTab="4" xr2:uid="{E1F56209-5FDF-9940-87DD-7244E19B7075}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Balanced" sheetId="2" r:id="rId2"/>
+    <sheet name="Low Fat" sheetId="7" r:id="rId3"/>
+    <sheet name="Low Carb" sheetId="8" r:id="rId4"/>
+    <sheet name="High Protein" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t>Age</t>
   </si>
@@ -63,6 +67,42 @@
   </si>
   <si>
     <t>Height cm</t>
+  </si>
+  <si>
+    <t>Calories</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t>Carbs</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Tracker</t>
+  </si>
+  <si>
+    <t>Food Item</t>
+  </si>
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>ONLY MODIFY A3 - D3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>DO NOT MODIFY!!</t>
   </si>
 </sst>
 </file>
@@ -74,7 +114,7 @@
     <numFmt numFmtId="165" formatCode="0\ &quot;lb&quot;"/>
     <numFmt numFmtId="166" formatCode="0\ &quot;cm&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,8 +129,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,8 +156,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -127,11 +186,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -156,6 +261,34 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,8 +607,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,4 +655,592 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABE6DD3-10F6-3142-8433-DC4524BEAAF2}">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="O1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F3" s="15"/>
+      <c r="O3">
+        <f>A3-SUMIFS($I$3:$I$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>B3-SUMIFS($J$3:$J$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>C3-SUMIFS($K$3:$K$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>D3-SUMIFS($L$3:$L$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{67684F61-11B8-024F-8C56-026B991D6867}">
+      <formula1>"Breakfast, Brunch, Lunch, Dinner, Snack"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D48D080-5560-5F47-947F-B10387429AB5}">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="O1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F3" s="15"/>
+      <c r="O3">
+        <f>A3-SUMIFS($I$3:$I$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>B3-SUMIFS($J$3:$J$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>C3-SUMIFS($K$3:$K$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>D3-SUMIFS($L$3:$L$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="O4:R4"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{0ED12C77-456A-1F45-9BD2-FC19F4E9F79F}">
+      <formula1>"Breakfast, Brunch, Lunch, Dinner, Snack"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A8BEDF-2513-7947-8462-BE2FCA99ADEB}">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="O1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F3" s="15"/>
+      <c r="O3">
+        <f>A3-SUMIFS($I$3:$I$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>B3-SUMIFS($J$3:$J$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>C3-SUMIFS($K$3:$K$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>D3-SUMIFS($L$3:$L$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="O4:R4"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{F78E8388-23BC-B04C-B4E7-E42384608FF3}">
+      <formula1>"Breakfast, Brunch, Lunch, Dinner, Snack"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5951C1D0-1A7B-3B49-927C-D967789B0DAC}">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="O1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F3" s="15"/>
+      <c r="O3">
+        <f>A3-SUMIFS($I$3:$I$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>B3-SUMIFS($J$3:$J$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>C3-SUMIFS($K$3:$K$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>D3-SUMIFS($L$3:$L$1000, $F$3:$F$1000, MAX($F$3:$F$1000))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="15"/>
+      <c r="O4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="O4:R4"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{1454FB38-1A5C-7F41-BFFE-9A7D3D8D1EDE}">
+      <formula1>"Breakfast, Brunch, Lunch, Dinner, Snack"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>